<commit_message>
NOJIRA: Fixing ForeignAccount suite
</commit_message>
<xml_diff>
--- a/ForeignAccountPayments/data/ForeignAccountScenarios.xlsx
+++ b/ForeignAccountPayments/data/ForeignAccountScenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EI11510\OneDrive - EVRY\SUITES\ForeignAccountPayments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ullasa\Projects\JenkinsRegression\V9_Master\V4\pr-regression-valuechain\ForeignAccountPayments\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586DD10C-D0C1-4B01-B7B9-90DE1C2B6E4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FF5654-F858-48B8-9FAE-D4A43EEFF0CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CF3585DE-88D5-44EA-8F24-D5664B0353CD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF3585DE-88D5-44EA-8F24-D5664B0353CD}"/>
   </bookViews>
   <sheets>
     <sheet name="ForeignAccountData" sheetId="1" r:id="rId1"/>
@@ -942,7 +942,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -963,12 +963,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1D1C1D"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -991,12 +985,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1311,61 +1304,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99167D2-1A67-4090-9DDA-43C23FBA3D58}">
-  <dimension ref="A1:ES23"/>
+  <dimension ref="A1:ES17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="AL15" sqref="AL15"/>
+    <sheetView tabSelected="1" topLeftCell="AC5" zoomScale="106" workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="54" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="12" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="12" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="25.42578125" customWidth="1"/>
-    <col min="53" max="53" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="25.44140625" customWidth="1"/>
+    <col min="53" max="53" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="16" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="23" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="28" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1814,7 +1807,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -1990,7 +1983,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2190,7 +2183,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2375,7 +2368,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="5" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2530,7 +2523,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2709,7 +2702,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2939,7 +2932,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -3115,7 +3108,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>199</v>
       </c>
@@ -3282,7 +3275,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -3440,7 +3433,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -3631,7 +3624,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -3789,7 +3782,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="13" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -4013,7 +4006,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -4168,7 +4161,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4323,7 +4316,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -4481,7 +4474,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="17" spans="1:149" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:149" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -4635,10 +4628,6 @@
       <c r="ES17" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="23" spans="1:149" x14ac:dyDescent="0.25">
-      <c r="W23" s="4"/>
-      <c r="CU23" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4648,6 +4637,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AE4DD9123F962F41835FC7D321FCB141" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="de6336216500a7e38ba084c9982896b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b0e30881-c016-458c-8507-45fc32ba8386" xmlns:ns4="5db95767-4948-4457-9bf0-58a2d914d66f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7410fb1a23a60d607d23e9ea1d96d6d8" ns3:_="" ns4:_="">
     <xsd:import namespace="b0e30881-c016-458c-8507-45fc32ba8386"/>
@@ -4858,15 +4856,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4874,6 +4863,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A17A79D-B9A5-4244-B479-1FAAAFD6DEA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDE33391-696A-4D77-AC08-AC151E4A1CA7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4888,14 +4885,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A17A79D-B9A5-4244-B479-1FAAAFD6DEA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
NOJIRA: Updated in FISK suite with valid POR scenarios.
</commit_message>
<xml_diff>
--- a/ForeignAccountPayments/data/ForeignAccountScenarios.xlsx
+++ b/ForeignAccountPayments/data/ForeignAccountScenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ullasa\Projects\JenkinsRegression\V9_Master\V4\pr-regression-valuechain\ForeignAccountPayments\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Evry Automation\latest\pr-regression-valuechain\ForeignAccountPayments\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FF5654-F858-48B8-9FAE-D4A43EEFF0CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DFEA1A-DEFC-4B0F-BABB-82FE735CD664}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF3585DE-88D5-44EA-8F24-D5664B0353CD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CF3585DE-88D5-44EA-8F24-D5664B0353CD}"/>
   </bookViews>
   <sheets>
     <sheet name="ForeignAccountData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="302">
   <si>
     <t>EVRYCPS</t>
   </si>
@@ -936,6 +936,9 @@
   </si>
   <si>
     <t>FDTR</t>
+  </si>
+  <si>
+    <t>28048100718</t>
   </si>
 </sst>
 </file>
@@ -965,12 +968,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -985,11 +994,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1306,59 +1317,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99167D2-1A67-4090-9DDA-43C23FBA3D58}">
   <dimension ref="A1:ES17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC5" zoomScale="106" workbookViewId="0">
-      <selection activeCell="AC16" sqref="AC16"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="Y6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="54" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="12" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="12" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="25.44140625" customWidth="1"/>
-    <col min="53" max="53" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="25.453125" customWidth="1"/>
+    <col min="53" max="53" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="16" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="23" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="31.08984375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="28" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="29.6328125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="32.6328125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="25.08984375" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="28.6328125" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="29.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1807,7 +1818,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -1983,7 +1994,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2194,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2368,7 +2379,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="5" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2427,7 +2438,7 @@
         <v>10000</v>
       </c>
       <c r="W5">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="X5" t="s">
         <v>12</v>
@@ -2444,8 +2455,8 @@
       <c r="AB5">
         <v>4201</v>
       </c>
-      <c r="AC5" s="3">
-        <v>926091891</v>
+      <c r="AC5" s="3" t="s">
+        <v>301</v>
       </c>
       <c r="AD5" t="s">
         <v>15</v>
@@ -2463,7 +2474,7 @@
         <v>20</v>
       </c>
       <c r="AI5">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AJ5" t="s">
         <v>195</v>
@@ -2493,7 +2504,7 @@
         <v>286</v>
       </c>
       <c r="AY5">
-        <v>32400033618</v>
+        <v>42010250514</v>
       </c>
       <c r="AZ5" t="s">
         <v>31</v>
@@ -2523,186 +2534,186 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:149" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:149" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>112233</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H6" t="b">
+      <c r="H6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="4">
         <v>0</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="4">
         <v>10000</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="4">
         <v>10000</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="4">
         <v>55057203187</v>
       </c>
-      <c r="X6" t="s">
+      <c r="X6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Y6" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="Z6" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="4">
         <v>2544</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="4">
         <v>2544</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AC6" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AE6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AF6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AG6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AH6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AI6">
+      <c r="AI6" s="4">
         <v>55057203187</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AP6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AQ6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AR6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AS6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="AW6" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="AY6">
-        <v>32400006297</v>
-      </c>
-      <c r="AZ6" t="s">
+      <c r="AY6" s="4">
+        <v>42010039950</v>
+      </c>
+      <c r="AZ6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="BA6" t="s">
+      <c r="BA6" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="BQ6" t="s">
+      <c r="BQ6" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="BR6">
+      <c r="BR6" s="4">
         <v>10</v>
       </c>
-      <c r="BT6" t="s">
+      <c r="BT6" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="BV6" t="s">
+      <c r="BV6" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="BW6" t="s">
+      <c r="BW6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="BZ6" t="s">
+      <c r="BZ6" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="CB6">
+      <c r="CB6" s="4">
         <v>10534</v>
       </c>
-      <c r="CC6" t="s">
+      <c r="CC6" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="CF6" t="s">
+      <c r="CF6" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="CG6" t="s">
+      <c r="CG6" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="CH6" t="s">
+      <c r="CH6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="CK6" t="s">
+      <c r="CK6" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="CM6">
+      <c r="CM6" s="4">
         <v>12930</v>
       </c>
-      <c r="CN6" t="s">
+      <c r="CN6" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="CP6" t="s">
+      <c r="CP6" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="CU6" t="s">
+      <c r="CU6" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="EQ6" t="s">
+      <c r="EQ6" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="ER6" t="s">
+      <c r="ER6" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="ES6" t="s">
+      <c r="ES6" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2932,7 +2943,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>199</v>
       </c>
@@ -3108,7 +3119,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>199</v>
       </c>
@@ -3275,7 +3286,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -3433,7 +3444,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -3492,7 +3503,7 @@
         <v>10000</v>
       </c>
       <c r="W11">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="X11" t="s">
         <v>12</v>
@@ -3510,7 +3521,7 @@
         <v>4201</v>
       </c>
       <c r="AC11">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AD11" t="s">
         <v>15</v>
@@ -3528,7 +3539,7 @@
         <v>20</v>
       </c>
       <c r="AI11">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AJ11" t="s">
         <v>195</v>
@@ -3555,7 +3566,7 @@
         <v>286</v>
       </c>
       <c r="AY11">
-        <v>32400033618</v>
+        <v>42010250514</v>
       </c>
       <c r="AZ11" t="s">
         <v>31</v>
@@ -3624,7 +3635,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -3683,7 +3694,7 @@
         <v>10000</v>
       </c>
       <c r="W12">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="X12" t="s">
         <v>12</v>
@@ -3701,7 +3712,7 @@
         <v>4201</v>
       </c>
       <c r="AC12">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AD12" t="s">
         <v>15</v>
@@ -3719,7 +3730,7 @@
         <v>20</v>
       </c>
       <c r="AI12">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AJ12" t="s">
         <v>195</v>
@@ -3749,7 +3760,7 @@
         <v>286</v>
       </c>
       <c r="AY12">
-        <v>32400033618</v>
+        <v>42010250514</v>
       </c>
       <c r="AZ12" t="s">
         <v>31</v>
@@ -3782,7 +3793,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="13" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -4006,7 +4017,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -4065,7 +4076,7 @@
         <v>10000</v>
       </c>
       <c r="W14">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="X14" t="s">
         <v>12</v>
@@ -4083,7 +4094,7 @@
         <v>4201</v>
       </c>
       <c r="AC14">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AD14" t="s">
         <v>15</v>
@@ -4101,7 +4112,7 @@
         <v>20</v>
       </c>
       <c r="AI14">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AJ14" t="s">
         <v>195</v>
@@ -4131,7 +4142,7 @@
         <v>286</v>
       </c>
       <c r="AY14">
-        <v>32400033618</v>
+        <v>42010250514</v>
       </c>
       <c r="AZ14" t="s">
         <v>31</v>
@@ -4161,7 +4172,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4220,7 +4231,7 @@
         <v>10000</v>
       </c>
       <c r="W15">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="X15" t="s">
         <v>12</v>
@@ -4238,7 +4249,7 @@
         <v>4201</v>
       </c>
       <c r="AC15">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AD15" t="s">
         <v>15</v>
@@ -4256,7 +4267,7 @@
         <v>20</v>
       </c>
       <c r="AI15">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AJ15" t="s">
         <v>195</v>
@@ -4286,7 +4297,7 @@
         <v>286</v>
       </c>
       <c r="AY15">
-        <v>32400033618</v>
+        <v>42010250514</v>
       </c>
       <c r="AZ15" t="s">
         <v>31</v>
@@ -4316,7 +4327,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -4375,7 +4386,7 @@
         <v>10000</v>
       </c>
       <c r="W16">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="X16" t="s">
         <v>12</v>
@@ -4393,7 +4404,7 @@
         <v>4201</v>
       </c>
       <c r="AC16">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AD16" t="s">
         <v>15</v>
@@ -4411,7 +4422,7 @@
         <v>20</v>
       </c>
       <c r="AI16">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AJ16" t="s">
         <v>195</v>
@@ -4441,7 +4452,7 @@
         <v>286</v>
       </c>
       <c r="AY16">
-        <v>32400033618</v>
+        <v>42010250514</v>
       </c>
       <c r="AZ16" t="s">
         <v>31</v>
@@ -4474,7 +4485,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="17" spans="1:149" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:149" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -4533,7 +4544,7 @@
         <v>10000</v>
       </c>
       <c r="W17">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="X17" t="s">
         <v>12</v>
@@ -4551,7 +4562,7 @@
         <v>4201</v>
       </c>
       <c r="AC17">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AD17" t="s">
         <v>15</v>
@@ -4569,7 +4580,7 @@
         <v>20</v>
       </c>
       <c r="AI17">
-        <v>926091891</v>
+        <v>28048100718</v>
       </c>
       <c r="AJ17" t="s">
         <v>195</v>
@@ -4599,7 +4610,7 @@
         <v>286</v>
       </c>
       <c r="AY17">
-        <v>32400033618</v>
+        <v>42010250514</v>
       </c>
       <c r="AZ17" t="s">
         <v>31</v>
@@ -4637,15 +4648,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AE4DD9123F962F41835FC7D321FCB141" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="de6336216500a7e38ba084c9982896b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b0e30881-c016-458c-8507-45fc32ba8386" xmlns:ns4="5db95767-4948-4457-9bf0-58a2d914d66f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7410fb1a23a60d607d23e9ea1d96d6d8" ns3:_="" ns4:_="">
     <xsd:import namespace="b0e30881-c016-458c-8507-45fc32ba8386"/>
@@ -4856,6 +4858,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4863,14 +4874,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A17A79D-B9A5-4244-B479-1FAAAFD6DEA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDE33391-696A-4D77-AC08-AC151E4A1CA7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4885,6 +4888,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A17A79D-B9A5-4244-B479-1FAAAFD6DEA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
NOJIRA: Updated in Foreign payment suite .
</commit_message>
<xml_diff>
--- a/ForeignAccountPayments/data/ForeignAccountScenarios.xlsx
+++ b/ForeignAccountPayments/data/ForeignAccountScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Evry Automation\latest\pr-regression-valuechain\ForeignAccountPayments\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DFEA1A-DEFC-4B0F-BABB-82FE735CD664}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452C6BD4-F9CB-4657-835C-03EA7BADA7C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CF3585DE-88D5-44EA-8F24-D5664B0353CD}"/>
   </bookViews>
@@ -1317,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99167D2-1A67-4090-9DDA-43C23FBA3D58}">
   <dimension ref="A1:ES17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="Y6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="AY6" sqref="AY6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4648,6 +4648,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AE4DD9123F962F41835FC7D321FCB141" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="de6336216500a7e38ba084c9982896b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b0e30881-c016-458c-8507-45fc32ba8386" xmlns:ns4="5db95767-4948-4457-9bf0-58a2d914d66f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7410fb1a23a60d607d23e9ea1d96d6d8" ns3:_="" ns4:_="">
     <xsd:import namespace="b0e30881-c016-458c-8507-45fc32ba8386"/>
@@ -4858,15 +4867,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4874,6 +4874,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A17A79D-B9A5-4244-B479-1FAAAFD6DEA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDE33391-696A-4D77-AC08-AC151E4A1CA7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4888,14 +4896,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A17A79D-B9A5-4244-B479-1FAAAFD6DEA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>